<commit_message>
TestCustomerAPI class added for end to end datadriven testing
</commit_message>
<xml_diff>
--- a/resources/SmartBytes_API_TestData.xlsx
+++ b/resources/SmartBytes_API_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamun/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamun/smartbytesRestAPI/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C029C322-CB04-8845-A52C-66AFC70A9972}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73A17CF-C0F0-9846-934D-55631B233FAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-71680" yWindow="2460" windowWidth="31120" windowHeight="17340" xr2:uid="{D4F74FA4-D23C-A34F-B9C4-0B171B8B10AC}"/>
+    <workbookView xWindow="-71680" yWindow="2460" windowWidth="31120" windowHeight="17340" activeTab="2" xr2:uid="{D4F74FA4-D23C-A34F-B9C4-0B171B8B10AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -118,15 +118,6 @@
     <t>Content Type</t>
   </si>
   <si>
-    <t>http://localhost:9090/api/customer/show?id=1</t>
-  </si>
-  <si>
-    <t>http://localhost:9090/api/customer/add</t>
-  </si>
-  <si>
-    <t>http://localhost:9090/api/customer/update/1</t>
-  </si>
-  <si>
     <t>Employee 1</t>
   </si>
   <si>
@@ -350,41 +341,50 @@
 }</t>
   </si>
   <si>
-    <t>http://localhost:9090/api/customer/delete/1</t>
-  </si>
-  <si>
     <t>Read country by iso code 2</t>
   </si>
   <si>
-    <t>http://localhost:9090/api/country/get/iso2code/IN</t>
-  </si>
-  <si>
-    <t>http://localhost:9090/api/country/get/iso3code/USA</t>
-  </si>
-  <si>
     <t>Read country by iso code 3-IND</t>
   </si>
   <si>
     <t>Read country by iso code 3-USA</t>
   </si>
   <si>
-    <t>http://localhost:9090/api/country/get/iso3code/IND</t>
-  </si>
-  <si>
     <t>Read customer 1</t>
   </si>
   <si>
     <t>Read customer 2</t>
   </si>
   <si>
-    <t>http://localhost:9090/api/customer/show?id=2</t>
+    <t>http://localhost:8080/api/customer/show?id=1</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/customer/show?id=2</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/customer/add</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/customer/update/1</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/customer/delete/1</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/country/get/iso2code/IN</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/country/get/iso3code/USA</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/country/get/iso3code/IND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -435,14 +435,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -541,7 +533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -551,7 +543,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -560,9 +551,9 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1132,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126173ED-5596-6043-A390-DE0D0F8526D3}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1146,32 +1137,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>77</v>
+      <c r="I1" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1181,26 +1172,26 @@
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>62</v>
+      <c r="C2" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F2" s="3">
         <v>48075</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1210,26 +1201,26 @@
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>63</v>
+      <c r="C3" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F3" s="3">
         <v>48076</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1239,26 +1230,26 @@
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>64</v>
+      <c r="C4" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F4" s="3">
         <v>48077</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1268,26 +1259,26 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>65</v>
+      <c r="C5" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F5" s="3">
         <v>48078</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1297,26 +1288,26 @@
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>66</v>
+      <c r="C6" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F6" s="3">
         <v>48079</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1326,26 +1317,26 @@
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>67</v>
+      <c r="C7" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F7" s="3">
         <v>48080</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1379,79 +1370,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="17">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="B3" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="17">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="B4" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="18">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="B5" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="17">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="18">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="C6" s="17">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="18">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="18">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="18">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <v>550</v>
       </c>
     </row>
@@ -1464,15 +1455,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0C1422-669F-204B-B9E3-9BBAADCB4E0B}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.83203125" style="7" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.6640625" style="7" customWidth="1"/>
     <col min="6" max="6" width="26.1640625" style="7" bestFit="1" customWidth="1"/>
@@ -1482,19 +1473,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>22</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -1507,185 +1498,185 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="19">
+      <c r="E2" s="9"/>
+      <c r="F2" s="18">
         <v>200</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>107</v>
+      <c r="B3" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="19">
+      <c r="E3" s="9"/>
+      <c r="F3" s="18">
         <v>200</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="F4" s="18">
+        <v>201</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" s="19">
-        <v>201</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="10"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="F5" s="18">
+        <v>200</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="19">
-        <v>200</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="10"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>96</v>
+      <c r="B6" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="19">
+      <c r="E6" s="10"/>
+      <c r="F6" s="18">
         <v>200</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="10"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>100</v>
+      <c r="B7" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9">
         <v>200</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>104</v>
+      <c r="B8" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9">
         <v>200</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="10"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>103</v>
+      <c r="B9" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9">
         <v>200</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="10"/>
+      <c r="H9" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1 A2:B2 A10:B1048576 A4:B7">
@@ -1781,6 +1772,7 @@
     <hyperlink ref="C8" r:id="rId5" xr:uid="{B122724E-EB7F-5649-B7D6-D352E127CA91}"/>
     <hyperlink ref="C9" r:id="rId6" xr:uid="{3CD6A4DA-43AA-1F4A-8BBC-13D5B3DB6E19}"/>
     <hyperlink ref="C3" r:id="rId7" xr:uid="{85F198F9-85D6-6E43-A6D7-42F3CD349093}"/>
+    <hyperlink ref="C4" r:id="rId8" xr:uid="{09ABDFAD-A847-BB40-908B-AEDDC50D01FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1832,122 +1824,122 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>